<commit_message>
ADM1 DAE implementation with pH solver
</commit_message>
<xml_diff>
--- a/qsdsan/data/_adm1.xlsx
+++ b/qsdsan/data/_adm1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\QSDsan\qsdsan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C0D3DA-85B9-4D25-B215-35B23BE3628C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ED38AB-2F30-49B0-96FC-F415066F0B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CCF55BD6-4F5E-4882-87DE-EFF69DB6A4AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="149">
   <si>
     <t>disintegration</t>
   </si>
@@ -335,30 +335,6 @@
     <t>1/(1 + S_h2/K_I_h2_j)</t>
   </si>
   <si>
-    <t>k_su * S_su/(K_su + S_su) * X_su</t>
-  </si>
-  <si>
-    <t>k_aa * S_aa/(K_aa + S_aa) * X_aa</t>
-  </si>
-  <si>
-    <t>k_fa * S_fa/(K_fa + S_fa) * X_fa</t>
-  </si>
-  <si>
-    <t>k_c4 * S_va/(K_va + S_va) * X_c4  * S_va/(S_va + S_bu)</t>
-  </si>
-  <si>
-    <t>k_c4 * S_bu/(K_bu + S_bu) * X_bu  * S_bu/(S_va + S_bu)</t>
-  </si>
-  <si>
-    <t>k_pro* S_pro/(K_pro + S_pro) * X_pro</t>
-  </si>
-  <si>
-    <t>k_ca* S_ac/(K_ac + S_ac) * X_ac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_h2* S_h2/(K_h2 + S_h2) * X_h2 </t>
-  </si>
-  <si>
     <t>I_pH</t>
   </si>
   <si>
@@ -483,6 +459,30 @@
   </si>
   <si>
     <t>K_c4</t>
+  </si>
+  <si>
+    <t>k_su * X_su * S_su/(K_su + S_su)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_aa * X_aa * S_aa/(K_aa + S_aa) </t>
+  </si>
+  <si>
+    <t>k_fa * X_fa * S_fa/(K_fa + S_fa)</t>
+  </si>
+  <si>
+    <t>k_c4 * X_c4 * S_va/(K_c4 + S_va) * S_va/(S_va + S_bu)</t>
+  </si>
+  <si>
+    <t>k_c4 * X_c4 * S_bu/(K_c4 + S_bu) * S_bu/(S_va + S_bu)</t>
+  </si>
+  <si>
+    <t>k_pro * X_pro * S_pro/(K_pro + S_pro)</t>
+  </si>
+  <si>
+    <t>k_h2 * X_h2 * S_h2/(K_h2 + S_h2)</t>
+  </si>
+  <si>
+    <t>k_ac * X_ac * S_ac/(K_ac + S_ac)</t>
   </si>
 </sst>
 </file>
@@ -838,7 +838,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
@@ -1374,7 +1374,7 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,6 +1465,12 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" t="s">
+        <v>60</v>
+      </c>
       <c r="M2" t="s">
         <v>60</v>
       </c>
@@ -1494,6 +1500,12 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
       <c r="O3">
         <v>-1</v>
       </c>
@@ -1508,6 +1520,12 @@
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>60</v>
+      </c>
       <c r="P4">
         <v>-1</v>
       </c>
@@ -1525,6 +1543,12 @@
       <c r="D5" t="s">
         <v>48</v>
       </c>
+      <c r="K5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" t="s">
+        <v>60</v>
+      </c>
       <c r="Q5">
         <v>-1</v>
       </c>
@@ -1561,7 +1585,7 @@
         <v>50</v>
       </c>
       <c r="Z6" t="s">
-        <v>99</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -1596,7 +1620,7 @@
         <v>53</v>
       </c>
       <c r="Z7" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1612,6 +1636,9 @@
       <c r="I8" t="s">
         <v>60</v>
       </c>
+      <c r="K8" t="s">
+        <v>60</v>
+      </c>
       <c r="L8" t="s">
         <v>60</v>
       </c>
@@ -1619,7 +1646,7 @@
         <v>54</v>
       </c>
       <c r="Z8" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -1638,6 +1665,9 @@
       <c r="I9" t="s">
         <v>60</v>
       </c>
+      <c r="K9" t="s">
+        <v>60</v>
+      </c>
       <c r="L9" t="s">
         <v>60</v>
       </c>
@@ -1645,7 +1675,7 @@
         <v>55</v>
       </c>
       <c r="Z9" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -1661,6 +1691,9 @@
       <c r="I10" t="s">
         <v>60</v>
       </c>
+      <c r="K10" t="s">
+        <v>60</v>
+      </c>
       <c r="L10" t="s">
         <v>60</v>
       </c>
@@ -1668,7 +1701,7 @@
         <v>55</v>
       </c>
       <c r="Z10" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -1694,7 +1727,7 @@
         <v>56</v>
       </c>
       <c r="Z11" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -1717,7 +1750,7 @@
         <v>51</v>
       </c>
       <c r="Z12" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -1740,13 +1773,19 @@
         <v>52</v>
       </c>
       <c r="Z13" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="K14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" t="s">
+        <v>60</v>
+      </c>
       <c r="N14">
         <v>1</v>
       </c>
@@ -1761,6 +1800,12 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="K15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" t="s">
+        <v>60</v>
+      </c>
       <c r="N15">
         <v>1</v>
       </c>
@@ -1775,6 +1820,12 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
       <c r="N16">
         <v>1</v>
       </c>
@@ -1789,6 +1840,12 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="K17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
       <c r="N17">
         <v>1</v>
       </c>
@@ -1803,6 +1860,12 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="K18" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
       <c r="N18">
         <v>1</v>
       </c>
@@ -1817,6 +1880,12 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
+      <c r="K19" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
       <c r="N19">
         <v>1</v>
       </c>
@@ -1831,6 +1900,12 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
+      <c r="K20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
       <c r="N20">
         <v>1</v>
       </c>
@@ -1855,7 +1930,7 @@
         <v>96</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I22">
         <v>0.4</v>
@@ -1875,7 +1950,7 @@
         <v>98</v>
       </c>
       <c r="H23" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I23">
         <v>0.25</v>
@@ -1889,16 +1964,16 @@
         <v>0.25</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G24" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H24" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I24">
         <v>0.2</v>
@@ -1915,10 +1990,10 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H25" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="I25">
         <v>0.1</v>
@@ -1935,10 +2010,10 @@
         <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H26" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I26">
         <v>30</v>
@@ -1946,13 +2021,13 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B27">
         <v>0.13</v>
       </c>
       <c r="H27" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I27">
         <v>0.5</v>
@@ -1960,16 +2035,16 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B28">
         <v>0.27</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="H28" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I28">
         <v>50</v>
@@ -1977,16 +2052,16 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B29">
         <v>0.41</v>
       </c>
       <c r="E29" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H29" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I29">
         <v>0.3</v>
@@ -1994,16 +2069,16 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B30">
         <v>0.23</v>
       </c>
       <c r="E30" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H30" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="I30">
         <v>6</v>
@@ -2011,16 +2086,16 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B31">
         <v>0.26</v>
       </c>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H31" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I31">
         <v>0.4</v>
@@ -2028,19 +2103,19 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B32">
         <v>0.05</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F32" s="1">
         <v>1E-4</v>
       </c>
       <c r="H32" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I32">
         <v>20</v>
@@ -2048,13 +2123,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B33">
         <v>0.4</v>
       </c>
       <c r="H33" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I33">
         <v>0.3</v>
@@ -2068,7 +2143,7 @@
         <v>0.7</v>
       </c>
       <c r="H34" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="I34">
         <v>13</v>
@@ -2082,7 +2157,7 @@
         <v>0.54</v>
       </c>
       <c r="H35" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I35">
         <v>0.3</v>
@@ -2096,7 +2171,7 @@
         <v>0.31</v>
       </c>
       <c r="H36" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I36">
         <v>8</v>
@@ -2110,7 +2185,7 @@
         <v>0.8</v>
       </c>
       <c r="H37" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I37">
         <v>0.15</v>
@@ -2124,7 +2199,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="H38" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="I38">
         <v>35</v>
@@ -2138,7 +2213,7 @@
         <v>0.1</v>
       </c>
       <c r="H39" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="I39" s="1">
         <v>2.5000000000000001E-5</v>
@@ -2152,7 +2227,7 @@
         <v>0.08</v>
       </c>
       <c r="H40" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I40">
         <v>0.02</v>
@@ -2166,7 +2241,7 @@
         <v>0.06</v>
       </c>
       <c r="H41" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I41">
         <v>0.02</v>
@@ -2180,7 +2255,7 @@
         <v>0.06</v>
       </c>
       <c r="H42" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I42">
         <v>0.02</v>
@@ -2194,7 +2269,7 @@
         <v>0.04</v>
       </c>
       <c r="H43" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I43">
         <v>0.02</v>
@@ -2208,7 +2283,7 @@
         <v>0.05</v>
       </c>
       <c r="H44" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="I44">
         <v>0.02</v>
@@ -2222,7 +2297,7 @@
         <v>0.06</v>
       </c>
       <c r="H45" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I45">
         <v>0.02</v>
@@ -2230,7 +2305,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I46">
         <v>0.02</v>

</xml_diff>